<commit_message>
update - capex proj events
</commit_message>
<xml_diff>
--- a/Capex/raw_data/RoughBook.xlsx
+++ b/Capex/raw_data/RoughBook.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iimv1-my.sharepoint.com/personal/kalyan_iimv_ac_in/Documents/Python-Exercise-KK/Kalyan-Jupyter-Notebooks/Capex/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{27E2263D-B2F9-2642-90FA-5A37E3A102DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4694233-86EF-434B-8533-28F6966F3D43}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{27E2263D-B2F9-2642-90FA-5A37E3A102DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD44EC34-F76B-3247-9FBD-D505629A3A91}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14600" activeTab="1" xr2:uid="{59470965-B567-3444-8030-BF238CF640B5}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14600" activeTab="2" xr2:uid="{59470965-B567-3444-8030-BF238CF640B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
     <sheet name="Full" sheetId="2" r:id="rId2"/>
+    <sheet name="Events" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="227">
   <si>
     <t>Non-financial</t>
   </si>
@@ -685,16 +686,55 @@
   </si>
   <si>
     <t>Ownership (All Owners) by State (India)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Project ABC</t>
+  </si>
+  <si>
+    <t>State Govt</t>
+  </si>
+  <si>
+    <t>Announced</t>
+  </si>
+  <si>
+    <t>Permission Receipt</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Project DEF</t>
+  </si>
+  <si>
+    <t>Pvt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -718,8 +758,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,7 +1243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBDCED2-B1A1-2643-B089-01F928A957B9}">
   <dimension ref="A1:A212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2271,4 +2313,117 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71C9095-FDD9-FC4B-B3B2-DDFF918E0B5B}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45056</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>